<commit_message>
Completed the Data Provider assignment
</commit_message>
<xml_diff>
--- a/JalaSeleniumAssignment/src/main/resources/includes/data.xlsx
+++ b/JalaSeleniumAssignment/src/main/resources/includes/data.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">abc123</t>
+    <t xml:space="preserve">admin123</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>